<commit_message>
Amélioration boutique + calculs dégâts
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -373,7 +373,7 @@
   <dimension ref="A1:AZ16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,7 +384,7 @@
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
       <c r="B1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -545,204 +545,204 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <f>$B$1*2</f>
+        <f>$B$1</f>
         <v>10</v>
       </c>
       <c r="D2">
         <f>C2+$B$1</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:AZ2" si="0">D2+$B$1</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F2">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H2">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="I2">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="J2">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="K2">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="L2">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="M2">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="N2">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="O2">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="P2">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="Q2">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="R2">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="S2">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="T2">
         <f t="shared" si="0"/>
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="U2">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>190</v>
       </c>
       <c r="V2">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>200</v>
       </c>
       <c r="W2">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="X2">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>220</v>
       </c>
       <c r="Y2">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>230</v>
       </c>
       <c r="Z2">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>240</v>
       </c>
       <c r="AA2">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="AB2">
         <f t="shared" si="0"/>
-        <v>135</v>
+        <v>260</v>
       </c>
       <c r="AC2">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>270</v>
       </c>
       <c r="AD2">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>280</v>
       </c>
       <c r="AE2">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>290</v>
       </c>
       <c r="AF2">
         <f t="shared" si="0"/>
-        <v>155</v>
+        <v>300</v>
       </c>
       <c r="AG2">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>310</v>
       </c>
       <c r="AH2">
         <f t="shared" si="0"/>
-        <v>165</v>
+        <v>320</v>
       </c>
       <c r="AI2">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>330</v>
       </c>
       <c r="AJ2">
         <f t="shared" si="0"/>
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AK2">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>350</v>
       </c>
       <c r="AL2">
         <f t="shared" si="0"/>
-        <v>185</v>
+        <v>360</v>
       </c>
       <c r="AM2">
         <f t="shared" si="0"/>
-        <v>190</v>
+        <v>370</v>
       </c>
       <c r="AN2">
         <f t="shared" si="0"/>
-        <v>195</v>
+        <v>380</v>
       </c>
       <c r="AO2">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>390</v>
       </c>
       <c r="AP2">
         <f t="shared" si="0"/>
-        <v>205</v>
+        <v>400</v>
       </c>
       <c r="AQ2">
         <f t="shared" si="0"/>
-        <v>210</v>
+        <v>410</v>
       </c>
       <c r="AR2">
         <f t="shared" si="0"/>
-        <v>215</v>
+        <v>420</v>
       </c>
       <c r="AS2">
         <f t="shared" si="0"/>
-        <v>220</v>
+        <v>430</v>
       </c>
       <c r="AT2">
         <f t="shared" si="0"/>
-        <v>225</v>
+        <v>440</v>
       </c>
       <c r="AU2">
         <f t="shared" si="0"/>
-        <v>230</v>
+        <v>450</v>
       </c>
       <c r="AV2">
         <f t="shared" si="0"/>
-        <v>235</v>
+        <v>460</v>
       </c>
       <c r="AW2">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>470</v>
       </c>
       <c r="AX2">
         <f t="shared" si="0"/>
-        <v>245</v>
+        <v>480</v>
       </c>
       <c r="AY2">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>490</v>
       </c>
       <c r="AZ2">
         <f t="shared" si="0"/>
-        <v>255</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.25">
@@ -758,199 +758,199 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:AZ7" si="1">ROUNDUP($A3*D$2,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F3">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H3">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I3">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J3">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="K3">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="L3">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="M3">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="N3">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="O3">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="P3">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="Q3">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="R3">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="S3">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="T3">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="U3">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="V3">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="W3">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="X3">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="Y3">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="Z3">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="AA3">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="AB3">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="AC3">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="AD3">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="AE3">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="AF3">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="AG3">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="AH3">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="AI3">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="AJ3">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="AK3">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="AL3">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="AM3">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="AN3">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="AO3">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="AP3">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="AQ3">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="AR3">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="AS3">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="AT3">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="AU3">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="AV3">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="AW3">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="AX3">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="AY3">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="AZ3">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.25">
@@ -966,199 +966,199 @@
       </c>
       <c r="D4">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H4">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="I4">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="J4">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="K4">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="L4">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="M4">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="N4">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="O4">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="P4">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="Q4">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="R4">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="S4">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="T4">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="U4">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="V4">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="W4">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="X4">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="Y4">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="Z4">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="AA4">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="AB4">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="AC4">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="AD4">
         <f t="shared" si="1"/>
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="AE4">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="AF4">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="AG4">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="AH4">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="AI4">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>132</v>
       </c>
       <c r="AJ4">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="AK4">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="AL4">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="AM4">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>148</v>
       </c>
       <c r="AN4">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>152</v>
       </c>
       <c r="AO4">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="AP4">
         <f t="shared" si="1"/>
-        <v>82</v>
+        <v>160</v>
       </c>
       <c r="AQ4">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>164</v>
       </c>
       <c r="AR4">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="AS4">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>172</v>
       </c>
       <c r="AT4">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>176</v>
       </c>
       <c r="AU4">
         <f t="shared" si="1"/>
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="AV4">
         <f t="shared" si="1"/>
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="AW4">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>188</v>
       </c>
       <c r="AX4">
         <f t="shared" si="1"/>
-        <v>98</v>
+        <v>192</v>
       </c>
       <c r="AY4">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>196</v>
       </c>
       <c r="AZ4">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
@@ -1174,199 +1174,199 @@
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="J5">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="N5">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="O5">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="P5">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="Q5">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="R5">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="S5">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="T5">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="U5">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="V5">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="W5">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>126</v>
       </c>
       <c r="X5">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>132</v>
       </c>
       <c r="Y5">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="Z5">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="AA5">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>150</v>
       </c>
       <c r="AB5">
         <f t="shared" si="1"/>
-        <v>81</v>
+        <v>156</v>
       </c>
       <c r="AC5">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>162</v>
       </c>
       <c r="AD5">
         <f t="shared" si="1"/>
-        <v>87</v>
+        <v>168</v>
       </c>
       <c r="AE5">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>174</v>
       </c>
       <c r="AF5">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>180</v>
       </c>
       <c r="AG5">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>186</v>
       </c>
       <c r="AH5">
         <f t="shared" si="1"/>
-        <v>99</v>
+        <v>192</v>
       </c>
       <c r="AI5">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>198</v>
       </c>
       <c r="AJ5">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>204</v>
       </c>
       <c r="AK5">
         <f t="shared" si="1"/>
-        <v>108</v>
+        <v>210</v>
       </c>
       <c r="AL5">
         <f t="shared" si="1"/>
-        <v>111</v>
+        <v>216</v>
       </c>
       <c r="AM5">
         <f t="shared" si="1"/>
-        <v>114</v>
+        <v>222</v>
       </c>
       <c r="AN5">
         <f t="shared" si="1"/>
-        <v>117</v>
+        <v>228</v>
       </c>
       <c r="AO5">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>234</v>
       </c>
       <c r="AP5">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>240</v>
       </c>
       <c r="AQ5">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>246</v>
       </c>
       <c r="AR5">
         <f t="shared" si="1"/>
-        <v>129</v>
+        <v>252</v>
       </c>
       <c r="AS5">
         <f t="shared" si="1"/>
-        <v>132</v>
+        <v>258</v>
       </c>
       <c r="AT5">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>264</v>
       </c>
       <c r="AU5">
         <f t="shared" si="1"/>
-        <v>138</v>
+        <v>270</v>
       </c>
       <c r="AV5">
         <f t="shared" si="1"/>
-        <v>141</v>
+        <v>276</v>
       </c>
       <c r="AW5">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>282</v>
       </c>
       <c r="AX5">
         <f t="shared" si="1"/>
-        <v>147</v>
+        <v>288</v>
       </c>
       <c r="AY5">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>294</v>
       </c>
       <c r="AZ5">
         <f t="shared" si="1"/>
-        <v>153</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
@@ -1382,199 +1382,199 @@
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="M6">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="N6">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="O6">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="P6">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="Q6">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="R6">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="S6">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="T6">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>144</v>
       </c>
       <c r="U6">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="V6">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>160</v>
       </c>
       <c r="W6">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>168</v>
       </c>
       <c r="X6">
         <f t="shared" si="1"/>
-        <v>92</v>
+        <v>176</v>
       </c>
       <c r="Y6">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>184</v>
       </c>
       <c r="Z6">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>192</v>
       </c>
       <c r="AA6">
         <f t="shared" si="1"/>
-        <v>104</v>
+        <v>200</v>
       </c>
       <c r="AB6">
         <f t="shared" si="1"/>
-        <v>108</v>
+        <v>208</v>
       </c>
       <c r="AC6">
         <f t="shared" si="1"/>
-        <v>112</v>
+        <v>216</v>
       </c>
       <c r="AD6">
         <f t="shared" si="1"/>
-        <v>116</v>
+        <v>224</v>
       </c>
       <c r="AE6">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>232</v>
       </c>
       <c r="AF6">
         <f t="shared" si="1"/>
-        <v>124</v>
+        <v>240</v>
       </c>
       <c r="AG6">
         <f t="shared" si="1"/>
-        <v>128</v>
+        <v>248</v>
       </c>
       <c r="AH6">
         <f t="shared" si="1"/>
-        <v>132</v>
+        <v>256</v>
       </c>
       <c r="AI6">
         <f t="shared" si="1"/>
-        <v>136</v>
+        <v>264</v>
       </c>
       <c r="AJ6">
         <f t="shared" si="1"/>
-        <v>140</v>
+        <v>272</v>
       </c>
       <c r="AK6">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>280</v>
       </c>
       <c r="AL6">
         <f t="shared" si="1"/>
-        <v>148</v>
+        <v>288</v>
       </c>
       <c r="AM6">
         <f t="shared" si="1"/>
-        <v>152</v>
+        <v>296</v>
       </c>
       <c r="AN6">
         <f t="shared" si="1"/>
-        <v>156</v>
+        <v>304</v>
       </c>
       <c r="AO6">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>312</v>
       </c>
       <c r="AP6">
         <f t="shared" si="1"/>
-        <v>164</v>
+        <v>320</v>
       </c>
       <c r="AQ6">
         <f t="shared" si="1"/>
-        <v>168</v>
+        <v>328</v>
       </c>
       <c r="AR6">
         <f t="shared" si="1"/>
-        <v>172</v>
+        <v>336</v>
       </c>
       <c r="AS6">
         <f t="shared" si="1"/>
-        <v>176</v>
+        <v>344</v>
       </c>
       <c r="AT6">
         <f t="shared" si="1"/>
-        <v>180</v>
+        <v>352</v>
       </c>
       <c r="AU6">
         <f t="shared" si="1"/>
-        <v>184</v>
+        <v>360</v>
       </c>
       <c r="AV6">
         <f t="shared" si="1"/>
-        <v>188</v>
+        <v>368</v>
       </c>
       <c r="AW6">
         <f t="shared" si="1"/>
-        <v>192</v>
+        <v>376</v>
       </c>
       <c r="AX6">
         <f t="shared" si="1"/>
-        <v>196</v>
+        <v>384</v>
       </c>
       <c r="AY6">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>392</v>
       </c>
       <c r="AZ6">
         <f t="shared" si="1"/>
-        <v>204</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
@@ -1590,199 +1590,199 @@
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="J7">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="L7">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="M7">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="O7">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="P7">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="Q7">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="R7">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="S7">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="T7">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="U7">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>190</v>
       </c>
       <c r="V7">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>200</v>
       </c>
       <c r="W7">
         <f t="shared" si="1"/>
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="X7">
         <f t="shared" si="1"/>
-        <v>115</v>
+        <v>220</v>
       </c>
       <c r="Y7">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>230</v>
       </c>
       <c r="Z7">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>240</v>
       </c>
       <c r="AA7">
         <f t="shared" si="1"/>
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="AB7">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>260</v>
       </c>
       <c r="AC7">
         <f t="shared" si="1"/>
-        <v>140</v>
+        <v>270</v>
       </c>
       <c r="AD7">
         <f t="shared" si="1"/>
-        <v>145</v>
+        <v>280</v>
       </c>
       <c r="AE7">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>290</v>
       </c>
       <c r="AF7">
         <f t="shared" si="1"/>
-        <v>155</v>
+        <v>300</v>
       </c>
       <c r="AG7">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>310</v>
       </c>
       <c r="AH7">
         <f t="shared" si="1"/>
-        <v>165</v>
+        <v>320</v>
       </c>
       <c r="AI7">
         <f t="shared" si="1"/>
-        <v>170</v>
+        <v>330</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="1"/>
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AK7">
         <f t="shared" si="1"/>
-        <v>180</v>
+        <v>350</v>
       </c>
       <c r="AL7">
         <f t="shared" si="1"/>
-        <v>185</v>
+        <v>360</v>
       </c>
       <c r="AM7">
         <f t="shared" si="1"/>
-        <v>190</v>
+        <v>370</v>
       </c>
       <c r="AN7">
         <f t="shared" si="1"/>
-        <v>195</v>
+        <v>380</v>
       </c>
       <c r="AO7">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>390</v>
       </c>
       <c r="AP7">
         <f t="shared" si="1"/>
-        <v>205</v>
+        <v>400</v>
       </c>
       <c r="AQ7">
         <f t="shared" si="1"/>
-        <v>210</v>
+        <v>410</v>
       </c>
       <c r="AR7">
         <f t="shared" si="1"/>
-        <v>215</v>
+        <v>420</v>
       </c>
       <c r="AS7">
         <f t="shared" si="1"/>
-        <v>220</v>
+        <v>430</v>
       </c>
       <c r="AT7">
         <f t="shared" si="1"/>
-        <v>225</v>
+        <v>440</v>
       </c>
       <c r="AU7">
         <f t="shared" si="1"/>
-        <v>230</v>
+        <v>450</v>
       </c>
       <c r="AV7">
         <f t="shared" si="1"/>
-        <v>235</v>
+        <v>460</v>
       </c>
       <c r="AW7">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>470</v>
       </c>
       <c r="AX7">
         <f t="shared" si="1"/>
-        <v>245</v>
+        <v>480</v>
       </c>
       <c r="AY7">
         <f t="shared" si="1"/>
-        <v>250</v>
+        <v>490</v>
       </c>
       <c r="AZ7">
         <f t="shared" si="1"/>
-        <v>255</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.25">
@@ -1949,203 +1949,203 @@
       </c>
       <c r="C11">
         <f>$B$1*2</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <f>C11+$B$1</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:AZ11" si="3">D11+$B$1</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F11">
         <f>E11+$B$1</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G11">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H11">
         <f t="shared" si="3"/>
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="I11">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="J11">
         <f t="shared" si="3"/>
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="K11">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="L11">
         <f t="shared" si="3"/>
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="M11">
         <f t="shared" si="3"/>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="N11">
         <f t="shared" si="3"/>
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="O11">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="P11">
         <f t="shared" si="3"/>
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="Q11">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="R11">
         <f t="shared" si="3"/>
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="S11">
         <f t="shared" si="3"/>
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="T11">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>190</v>
       </c>
       <c r="U11">
         <f t="shared" si="3"/>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="V11">
         <f t="shared" si="3"/>
-        <v>105</v>
+        <v>210</v>
       </c>
       <c r="W11">
         <f t="shared" si="3"/>
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="X11">
         <f t="shared" si="3"/>
-        <v>115</v>
+        <v>230</v>
       </c>
       <c r="Y11">
         <f t="shared" si="3"/>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="Z11">
         <f t="shared" si="3"/>
-        <v>125</v>
+        <v>250</v>
       </c>
       <c r="AA11">
         <f t="shared" si="3"/>
-        <v>130</v>
+        <v>260</v>
       </c>
       <c r="AB11">
         <f t="shared" si="3"/>
-        <v>135</v>
+        <v>270</v>
       </c>
       <c r="AC11">
         <f t="shared" si="3"/>
-        <v>140</v>
+        <v>280</v>
       </c>
       <c r="AD11">
         <f t="shared" si="3"/>
-        <v>145</v>
+        <v>290</v>
       </c>
       <c r="AE11">
         <f t="shared" si="3"/>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="AF11">
         <f t="shared" si="3"/>
-        <v>155</v>
+        <v>310</v>
       </c>
       <c r="AG11">
         <f t="shared" si="3"/>
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="AH11">
         <f t="shared" si="3"/>
-        <v>165</v>
+        <v>330</v>
       </c>
       <c r="AI11">
         <f t="shared" si="3"/>
-        <v>170</v>
+        <v>340</v>
       </c>
       <c r="AJ11">
         <f t="shared" si="3"/>
-        <v>175</v>
+        <v>350</v>
       </c>
       <c r="AK11">
         <f t="shared" si="3"/>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="AL11">
         <f t="shared" si="3"/>
-        <v>185</v>
+        <v>370</v>
       </c>
       <c r="AM11">
         <f t="shared" si="3"/>
-        <v>190</v>
+        <v>380</v>
       </c>
       <c r="AN11">
         <f t="shared" si="3"/>
-        <v>195</v>
+        <v>390</v>
       </c>
       <c r="AO11">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="AP11">
         <f t="shared" si="3"/>
-        <v>205</v>
+        <v>410</v>
       </c>
       <c r="AQ11">
         <f t="shared" si="3"/>
-        <v>210</v>
+        <v>420</v>
       </c>
       <c r="AR11">
         <f t="shared" si="3"/>
-        <v>215</v>
+        <v>430</v>
       </c>
       <c r="AS11">
         <f t="shared" si="3"/>
-        <v>220</v>
+        <v>440</v>
       </c>
       <c r="AT11">
         <f t="shared" si="3"/>
-        <v>225</v>
+        <v>450</v>
       </c>
       <c r="AU11">
         <f t="shared" si="3"/>
-        <v>230</v>
+        <v>460</v>
       </c>
       <c r="AV11">
         <f t="shared" si="3"/>
-        <v>235</v>
+        <v>470</v>
       </c>
       <c r="AW11">
         <f t="shared" si="3"/>
-        <v>240</v>
+        <v>480</v>
       </c>
       <c r="AX11">
         <f t="shared" si="3"/>
-        <v>245</v>
+        <v>490</v>
       </c>
       <c r="AY11">
         <f t="shared" si="3"/>
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="AZ11">
         <f t="shared" si="3"/>
-        <v>255</v>
+        <v>510</v>
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.25">
@@ -2161,199 +2161,199 @@
       </c>
       <c r="D12">
         <f t="shared" ref="D12:AZ16" si="4">ROUNDUP($A12*D$2,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E12">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F12">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G12">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H12">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I12">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J12">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="K12">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="L12">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="M12">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="N12">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="O12">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="P12">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="Q12">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="R12">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="S12">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="T12">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="U12">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="V12">
         <f t="shared" si="4"/>
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="W12">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="X12">
         <f t="shared" si="4"/>
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="Y12">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="Z12">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="AA12">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="AB12">
         <f t="shared" si="4"/>
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="AC12">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="AD12">
         <f t="shared" si="4"/>
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="AE12">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="AF12">
         <f t="shared" si="4"/>
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="AG12">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="AH12">
         <f t="shared" si="4"/>
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="AI12">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="AJ12">
         <f t="shared" si="4"/>
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="AK12">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="AL12">
         <f t="shared" si="4"/>
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="AM12">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="AN12">
         <f t="shared" si="4"/>
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="AO12">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="AP12">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="AQ12">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="AR12">
         <f t="shared" si="4"/>
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="AS12">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="AT12">
         <f t="shared" si="4"/>
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="AU12">
         <f t="shared" si="4"/>
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="AV12">
         <f t="shared" si="4"/>
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="AW12">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="AX12">
         <f t="shared" si="4"/>
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="AY12">
         <f t="shared" si="4"/>
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="AZ12">
         <f t="shared" si="4"/>
-        <v>51</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.25">
@@ -2369,199 +2369,199 @@
       </c>
       <c r="D13">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E13">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F13">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G13">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H13">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="I13">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="J13">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="K13">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="L13">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="M13">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="N13">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="O13">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="P13">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="Q13">
         <f t="shared" si="5"/>
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="R13">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="S13">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="T13">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="U13">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="V13">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="W13">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="X13">
         <f t="shared" si="4"/>
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="Y13">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="Z13">
         <f t="shared" si="4"/>
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="AA13">
         <f t="shared" si="4"/>
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="AB13">
         <f t="shared" si="4"/>
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="AC13">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="AD13">
         <f t="shared" si="4"/>
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="AE13">
         <f t="shared" si="4"/>
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="AF13">
         <f t="shared" si="4"/>
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="AG13">
         <f t="shared" si="4"/>
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="AH13">
         <f t="shared" si="4"/>
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="AI13">
         <f t="shared" si="4"/>
-        <v>68</v>
+        <v>132</v>
       </c>
       <c r="AJ13">
         <f t="shared" si="4"/>
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="AK13">
         <f t="shared" si="4"/>
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="AL13">
         <f t="shared" si="4"/>
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="AM13">
         <f t="shared" si="4"/>
-        <v>76</v>
+        <v>148</v>
       </c>
       <c r="AN13">
         <f t="shared" si="4"/>
-        <v>78</v>
+        <v>152</v>
       </c>
       <c r="AO13">
         <f t="shared" si="4"/>
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="AP13">
         <f t="shared" si="4"/>
-        <v>82</v>
+        <v>160</v>
       </c>
       <c r="AQ13">
         <f t="shared" si="4"/>
-        <v>84</v>
+        <v>164</v>
       </c>
       <c r="AR13">
         <f t="shared" si="4"/>
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="AS13">
         <f t="shared" si="4"/>
-        <v>88</v>
+        <v>172</v>
       </c>
       <c r="AT13">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>176</v>
       </c>
       <c r="AU13">
         <f t="shared" si="4"/>
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="AV13">
         <f t="shared" si="4"/>
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="AW13">
         <f t="shared" si="4"/>
-        <v>96</v>
+        <v>188</v>
       </c>
       <c r="AX13">
         <f t="shared" si="4"/>
-        <v>98</v>
+        <v>192</v>
       </c>
       <c r="AY13">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>196</v>
       </c>
       <c r="AZ13">
         <f t="shared" si="4"/>
-        <v>102</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.25">
@@ -2577,199 +2577,199 @@
       </c>
       <c r="D14">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E14">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F14">
         <f>ROUNDUP($A14*F$2,0)</f>
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G14">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H14">
         <f t="shared" si="4"/>
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="I14">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="J14">
         <f t="shared" si="4"/>
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="K14">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="L14">
         <f t="shared" si="4"/>
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="M14">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="N14">
         <f t="shared" si="4"/>
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="O14">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="P14">
         <f t="shared" si="4"/>
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="Q14">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="R14">
         <f t="shared" si="4"/>
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="S14">
         <f t="shared" si="4"/>
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="T14">
         <f t="shared" si="4"/>
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="U14">
         <f t="shared" si="4"/>
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="V14">
         <f t="shared" si="4"/>
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="W14">
         <f t="shared" si="4"/>
-        <v>66</v>
+        <v>126</v>
       </c>
       <c r="X14">
         <f t="shared" si="4"/>
-        <v>69</v>
+        <v>132</v>
       </c>
       <c r="Y14">
         <f t="shared" si="4"/>
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="Z14">
         <f t="shared" si="4"/>
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="AA14">
         <f t="shared" si="4"/>
-        <v>78</v>
+        <v>150</v>
       </c>
       <c r="AB14">
         <f t="shared" si="4"/>
-        <v>81</v>
+        <v>156</v>
       </c>
       <c r="AC14">
         <f t="shared" si="4"/>
-        <v>84</v>
+        <v>162</v>
       </c>
       <c r="AD14">
         <f t="shared" si="4"/>
-        <v>87</v>
+        <v>168</v>
       </c>
       <c r="AE14">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>174</v>
       </c>
       <c r="AF14">
         <f t="shared" si="4"/>
-        <v>93</v>
+        <v>180</v>
       </c>
       <c r="AG14">
         <f t="shared" si="4"/>
-        <v>96</v>
+        <v>186</v>
       </c>
       <c r="AH14">
         <f t="shared" si="4"/>
-        <v>99</v>
+        <v>192</v>
       </c>
       <c r="AI14">
         <f t="shared" si="4"/>
-        <v>102</v>
+        <v>198</v>
       </c>
       <c r="AJ14">
         <f t="shared" si="4"/>
-        <v>105</v>
+        <v>204</v>
       </c>
       <c r="AK14">
         <f t="shared" si="4"/>
-        <v>108</v>
+        <v>210</v>
       </c>
       <c r="AL14">
         <f t="shared" si="4"/>
-        <v>111</v>
+        <v>216</v>
       </c>
       <c r="AM14">
         <f t="shared" si="4"/>
-        <v>114</v>
+        <v>222</v>
       </c>
       <c r="AN14">
         <f t="shared" si="4"/>
-        <v>117</v>
+        <v>228</v>
       </c>
       <c r="AO14">
         <f t="shared" si="4"/>
-        <v>120</v>
+        <v>234</v>
       </c>
       <c r="AP14">
         <f t="shared" si="4"/>
-        <v>123</v>
+        <v>240</v>
       </c>
       <c r="AQ14">
         <f t="shared" si="4"/>
-        <v>126</v>
+        <v>246</v>
       </c>
       <c r="AR14">
         <f t="shared" si="4"/>
-        <v>129</v>
+        <v>252</v>
       </c>
       <c r="AS14">
         <f t="shared" si="4"/>
-        <v>132</v>
+        <v>258</v>
       </c>
       <c r="AT14">
         <f t="shared" si="4"/>
-        <v>135</v>
+        <v>264</v>
       </c>
       <c r="AU14">
         <f t="shared" si="4"/>
-        <v>138</v>
+        <v>270</v>
       </c>
       <c r="AV14">
         <f t="shared" si="4"/>
-        <v>141</v>
+        <v>276</v>
       </c>
       <c r="AW14">
         <f t="shared" si="4"/>
-        <v>144</v>
+        <v>282</v>
       </c>
       <c r="AX14">
         <f t="shared" si="4"/>
-        <v>147</v>
+        <v>288</v>
       </c>
       <c r="AY14">
         <f t="shared" si="4"/>
-        <v>150</v>
+        <v>294</v>
       </c>
       <c r="AZ14">
         <f t="shared" si="4"/>
-        <v>153</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.25">
@@ -2785,199 +2785,199 @@
       </c>
       <c r="D15">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E15">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F15">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="G15">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="H15">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="I15">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="J15">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="K15">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="L15">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="M15">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="N15">
         <f t="shared" si="4"/>
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="O15">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="P15">
         <f t="shared" si="4"/>
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="Q15">
         <f t="shared" si="4"/>
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="R15">
         <f t="shared" si="4"/>
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="S15">
         <f t="shared" si="4"/>
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="T15">
         <f t="shared" si="4"/>
-        <v>76</v>
+        <v>144</v>
       </c>
       <c r="U15">
         <f t="shared" si="4"/>
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="V15">
         <f t="shared" si="4"/>
-        <v>84</v>
+        <v>160</v>
       </c>
       <c r="W15">
         <f t="shared" si="4"/>
-        <v>88</v>
+        <v>168</v>
       </c>
       <c r="X15">
         <f t="shared" si="4"/>
-        <v>92</v>
+        <v>176</v>
       </c>
       <c r="Y15">
         <f t="shared" si="4"/>
-        <v>96</v>
+        <v>184</v>
       </c>
       <c r="Z15">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>192</v>
       </c>
       <c r="AA15">
         <f t="shared" si="4"/>
-        <v>104</v>
+        <v>200</v>
       </c>
       <c r="AB15">
         <f t="shared" si="4"/>
-        <v>108</v>
+        <v>208</v>
       </c>
       <c r="AC15">
         <f t="shared" si="4"/>
-        <v>112</v>
+        <v>216</v>
       </c>
       <c r="AD15">
         <f t="shared" si="4"/>
-        <v>116</v>
+        <v>224</v>
       </c>
       <c r="AE15">
         <f t="shared" si="4"/>
-        <v>120</v>
+        <v>232</v>
       </c>
       <c r="AF15">
         <f t="shared" si="4"/>
-        <v>124</v>
+        <v>240</v>
       </c>
       <c r="AG15">
         <f t="shared" si="4"/>
-        <v>128</v>
+        <v>248</v>
       </c>
       <c r="AH15">
         <f t="shared" si="4"/>
-        <v>132</v>
+        <v>256</v>
       </c>
       <c r="AI15">
         <f t="shared" si="4"/>
-        <v>136</v>
+        <v>264</v>
       </c>
       <c r="AJ15">
         <f t="shared" si="4"/>
-        <v>140</v>
+        <v>272</v>
       </c>
       <c r="AK15">
         <f t="shared" si="4"/>
-        <v>144</v>
+        <v>280</v>
       </c>
       <c r="AL15">
         <f t="shared" si="4"/>
-        <v>148</v>
+        <v>288</v>
       </c>
       <c r="AM15">
         <f t="shared" si="4"/>
-        <v>152</v>
+        <v>296</v>
       </c>
       <c r="AN15">
         <f t="shared" si="4"/>
-        <v>156</v>
+        <v>304</v>
       </c>
       <c r="AO15">
         <f t="shared" si="4"/>
-        <v>160</v>
+        <v>312</v>
       </c>
       <c r="AP15">
         <f t="shared" si="4"/>
-        <v>164</v>
+        <v>320</v>
       </c>
       <c r="AQ15">
         <f t="shared" si="4"/>
-        <v>168</v>
+        <v>328</v>
       </c>
       <c r="AR15">
         <f t="shared" si="4"/>
-        <v>172</v>
+        <v>336</v>
       </c>
       <c r="AS15">
         <f t="shared" si="4"/>
-        <v>176</v>
+        <v>344</v>
       </c>
       <c r="AT15">
         <f t="shared" si="4"/>
-        <v>180</v>
+        <v>352</v>
       </c>
       <c r="AU15">
         <f t="shared" si="4"/>
-        <v>184</v>
+        <v>360</v>
       </c>
       <c r="AV15">
         <f t="shared" si="4"/>
-        <v>188</v>
+        <v>368</v>
       </c>
       <c r="AW15">
         <f t="shared" si="4"/>
-        <v>192</v>
+        <v>376</v>
       </c>
       <c r="AX15">
         <f t="shared" si="4"/>
-        <v>196</v>
+        <v>384</v>
       </c>
       <c r="AY15">
         <f t="shared" si="4"/>
-        <v>200</v>
+        <v>392</v>
       </c>
       <c r="AZ15">
         <f t="shared" si="4"/>
-        <v>204</v>
+        <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.25">
@@ -2993,199 +2993,199 @@
       </c>
       <c r="D16">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E16">
         <f>ROUNDUP($A16*E$2,0)</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F16">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G16">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H16">
         <f t="shared" si="4"/>
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="I16">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="J16">
         <f t="shared" si="4"/>
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="K16">
         <f t="shared" si="4"/>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="L16">
         <f t="shared" si="4"/>
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="M16">
         <f t="shared" si="4"/>
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="N16">
         <f t="shared" si="4"/>
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="O16">
         <f t="shared" si="4"/>
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="P16">
         <f t="shared" si="4"/>
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="Q16">
         <f t="shared" si="4"/>
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="R16">
         <f t="shared" si="4"/>
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="S16">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="T16">
         <f t="shared" si="4"/>
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="U16">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>190</v>
       </c>
       <c r="V16">
         <f t="shared" si="4"/>
-        <v>105</v>
+        <v>200</v>
       </c>
       <c r="W16">
         <f t="shared" si="4"/>
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="X16">
         <f t="shared" si="4"/>
-        <v>115</v>
+        <v>220</v>
       </c>
       <c r="Y16">
         <f t="shared" si="4"/>
-        <v>120</v>
+        <v>230</v>
       </c>
       <c r="Z16">
         <f t="shared" si="4"/>
-        <v>125</v>
+        <v>240</v>
       </c>
       <c r="AA16">
         <f t="shared" si="4"/>
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="AB16">
         <f t="shared" si="4"/>
-        <v>135</v>
+        <v>260</v>
       </c>
       <c r="AC16">
         <f t="shared" si="4"/>
-        <v>140</v>
+        <v>270</v>
       </c>
       <c r="AD16">
         <f t="shared" si="4"/>
-        <v>145</v>
+        <v>280</v>
       </c>
       <c r="AE16">
         <f t="shared" si="4"/>
-        <v>150</v>
+        <v>290</v>
       </c>
       <c r="AF16">
         <f t="shared" si="4"/>
-        <v>155</v>
+        <v>300</v>
       </c>
       <c r="AG16">
         <f t="shared" si="4"/>
-        <v>160</v>
+        <v>310</v>
       </c>
       <c r="AH16">
         <f t="shared" si="4"/>
-        <v>165</v>
+        <v>320</v>
       </c>
       <c r="AI16">
         <f t="shared" si="4"/>
-        <v>170</v>
+        <v>330</v>
       </c>
       <c r="AJ16">
         <f t="shared" si="4"/>
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AK16">
         <f t="shared" si="4"/>
-        <v>180</v>
+        <v>350</v>
       </c>
       <c r="AL16">
         <f t="shared" si="4"/>
-        <v>185</v>
+        <v>360</v>
       </c>
       <c r="AM16">
         <f t="shared" si="4"/>
-        <v>190</v>
+        <v>370</v>
       </c>
       <c r="AN16">
         <f t="shared" si="4"/>
-        <v>195</v>
+        <v>380</v>
       </c>
       <c r="AO16">
         <f t="shared" si="4"/>
-        <v>200</v>
+        <v>390</v>
       </c>
       <c r="AP16">
         <f t="shared" si="4"/>
-        <v>205</v>
+        <v>400</v>
       </c>
       <c r="AQ16">
         <f t="shared" si="4"/>
-        <v>210</v>
+        <v>410</v>
       </c>
       <c r="AR16">
         <f t="shared" si="4"/>
-        <v>215</v>
+        <v>420</v>
       </c>
       <c r="AS16">
         <f t="shared" si="4"/>
-        <v>220</v>
+        <v>430</v>
       </c>
       <c r="AT16">
         <f t="shared" si="4"/>
-        <v>225</v>
+        <v>440</v>
       </c>
       <c r="AU16">
         <f t="shared" si="4"/>
-        <v>230</v>
+        <v>450</v>
       </c>
       <c r="AV16">
         <f t="shared" si="4"/>
-        <v>235</v>
+        <v>460</v>
       </c>
       <c r="AW16">
         <f t="shared" si="4"/>
-        <v>240</v>
+        <v>470</v>
       </c>
       <c r="AX16">
         <f t="shared" si="4"/>
-        <v>245</v>
+        <v>480</v>
       </c>
       <c r="AY16">
         <f t="shared" si="4"/>
-        <v>250</v>
+        <v>490</v>
       </c>
       <c r="AZ16">
         <f t="shared" si="4"/>
-        <v>255</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Affichage salon carte hero
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -373,7 +373,7 @@
   <dimension ref="A1:AZ16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,7 +384,7 @@
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
       <c r="B1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -545,204 +545,204 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <f>$B$1*2</f>
+        <f>$B$1</f>
         <v>10</v>
       </c>
       <c r="D2">
         <f>C2+$B$1</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:AZ2" si="0">D2+$B$1</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F2">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H2">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="I2">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="J2">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="K2">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="L2">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="M2">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="N2">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="O2">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="P2">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="Q2">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="R2">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="S2">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="T2">
         <f t="shared" si="0"/>
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="U2">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>190</v>
       </c>
       <c r="V2">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>200</v>
       </c>
       <c r="W2">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="X2">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>220</v>
       </c>
       <c r="Y2">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>230</v>
       </c>
       <c r="Z2">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>240</v>
       </c>
       <c r="AA2">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="AB2">
         <f t="shared" si="0"/>
-        <v>135</v>
+        <v>260</v>
       </c>
       <c r="AC2">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>270</v>
       </c>
       <c r="AD2">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>280</v>
       </c>
       <c r="AE2">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>290</v>
       </c>
       <c r="AF2">
         <f t="shared" si="0"/>
-        <v>155</v>
+        <v>300</v>
       </c>
       <c r="AG2">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>310</v>
       </c>
       <c r="AH2">
         <f t="shared" si="0"/>
-        <v>165</v>
+        <v>320</v>
       </c>
       <c r="AI2">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>330</v>
       </c>
       <c r="AJ2">
         <f t="shared" si="0"/>
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AK2">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>350</v>
       </c>
       <c r="AL2">
         <f t="shared" si="0"/>
-        <v>185</v>
+        <v>360</v>
       </c>
       <c r="AM2">
         <f t="shared" si="0"/>
-        <v>190</v>
+        <v>370</v>
       </c>
       <c r="AN2">
         <f t="shared" si="0"/>
-        <v>195</v>
+        <v>380</v>
       </c>
       <c r="AO2">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>390</v>
       </c>
       <c r="AP2">
         <f t="shared" si="0"/>
-        <v>205</v>
+        <v>400</v>
       </c>
       <c r="AQ2">
         <f t="shared" si="0"/>
-        <v>210</v>
+        <v>410</v>
       </c>
       <c r="AR2">
         <f t="shared" si="0"/>
-        <v>215</v>
+        <v>420</v>
       </c>
       <c r="AS2">
         <f t="shared" si="0"/>
-        <v>220</v>
+        <v>430</v>
       </c>
       <c r="AT2">
         <f t="shared" si="0"/>
-        <v>225</v>
+        <v>440</v>
       </c>
       <c r="AU2">
         <f t="shared" si="0"/>
-        <v>230</v>
+        <v>450</v>
       </c>
       <c r="AV2">
         <f t="shared" si="0"/>
-        <v>235</v>
+        <v>460</v>
       </c>
       <c r="AW2">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>470</v>
       </c>
       <c r="AX2">
         <f t="shared" si="0"/>
-        <v>245</v>
+        <v>480</v>
       </c>
       <c r="AY2">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>490</v>
       </c>
       <c r="AZ2">
         <f t="shared" si="0"/>
-        <v>255</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.25">
@@ -758,199 +758,199 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:AZ7" si="1">ROUNDUP($A3*D$2,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F3">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H3">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I3">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J3">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="K3">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="L3">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="M3">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="N3">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="O3">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="P3">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="Q3">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="R3">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="S3">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="T3">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="U3">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="V3">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="W3">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="X3">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="Y3">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="Z3">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="AA3">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="AB3">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="AC3">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="AD3">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="AE3">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="AF3">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="AG3">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="AH3">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="AI3">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="AJ3">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="AK3">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="AL3">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="AM3">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="AN3">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="AO3">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="AP3">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="AQ3">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="AR3">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="AS3">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="AT3">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="AU3">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="AV3">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="AW3">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="AX3">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="AY3">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="AZ3">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.25">
@@ -966,199 +966,199 @@
       </c>
       <c r="D4">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H4">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="I4">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="J4">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="K4">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="L4">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="M4">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="N4">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="O4">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="P4">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="Q4">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="R4">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="S4">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="T4">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="U4">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="V4">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="W4">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="X4">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="Y4">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="Z4">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="AA4">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="AB4">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="AC4">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="AD4">
         <f t="shared" si="1"/>
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="AE4">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="AF4">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="AG4">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="AH4">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="AI4">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>132</v>
       </c>
       <c r="AJ4">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="AK4">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="AL4">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="AM4">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>148</v>
       </c>
       <c r="AN4">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>152</v>
       </c>
       <c r="AO4">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="AP4">
         <f t="shared" si="1"/>
-        <v>82</v>
+        <v>160</v>
       </c>
       <c r="AQ4">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>164</v>
       </c>
       <c r="AR4">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="AS4">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>172</v>
       </c>
       <c r="AT4">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>176</v>
       </c>
       <c r="AU4">
         <f t="shared" si="1"/>
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="AV4">
         <f t="shared" si="1"/>
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="AW4">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>188</v>
       </c>
       <c r="AX4">
         <f t="shared" si="1"/>
-        <v>98</v>
+        <v>192</v>
       </c>
       <c r="AY4">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>196</v>
       </c>
       <c r="AZ4">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
@@ -1174,199 +1174,199 @@
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="J5">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="N5">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="O5">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="P5">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="Q5">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="R5">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="S5">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="T5">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="U5">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="V5">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="W5">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>126</v>
       </c>
       <c r="X5">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>132</v>
       </c>
       <c r="Y5">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="Z5">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="AA5">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>150</v>
       </c>
       <c r="AB5">
         <f t="shared" si="1"/>
-        <v>81</v>
+        <v>156</v>
       </c>
       <c r="AC5">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>162</v>
       </c>
       <c r="AD5">
         <f t="shared" si="1"/>
-        <v>87</v>
+        <v>168</v>
       </c>
       <c r="AE5">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>174</v>
       </c>
       <c r="AF5">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>180</v>
       </c>
       <c r="AG5">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>186</v>
       </c>
       <c r="AH5">
         <f t="shared" si="1"/>
-        <v>99</v>
+        <v>192</v>
       </c>
       <c r="AI5">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>198</v>
       </c>
       <c r="AJ5">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>204</v>
       </c>
       <c r="AK5">
         <f t="shared" si="1"/>
-        <v>108</v>
+        <v>210</v>
       </c>
       <c r="AL5">
         <f t="shared" si="1"/>
-        <v>111</v>
+        <v>216</v>
       </c>
       <c r="AM5">
         <f t="shared" si="1"/>
-        <v>114</v>
+        <v>222</v>
       </c>
       <c r="AN5">
         <f t="shared" si="1"/>
-        <v>117</v>
+        <v>228</v>
       </c>
       <c r="AO5">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>234</v>
       </c>
       <c r="AP5">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>240</v>
       </c>
       <c r="AQ5">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>246</v>
       </c>
       <c r="AR5">
         <f t="shared" si="1"/>
-        <v>129</v>
+        <v>252</v>
       </c>
       <c r="AS5">
         <f t="shared" si="1"/>
-        <v>132</v>
+        <v>258</v>
       </c>
       <c r="AT5">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>264</v>
       </c>
       <c r="AU5">
         <f t="shared" si="1"/>
-        <v>138</v>
+        <v>270</v>
       </c>
       <c r="AV5">
         <f t="shared" si="1"/>
-        <v>141</v>
+        <v>276</v>
       </c>
       <c r="AW5">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>282</v>
       </c>
       <c r="AX5">
         <f t="shared" si="1"/>
-        <v>147</v>
+        <v>288</v>
       </c>
       <c r="AY5">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>294</v>
       </c>
       <c r="AZ5">
         <f t="shared" si="1"/>
-        <v>153</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
@@ -1382,199 +1382,199 @@
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="M6">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="N6">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="O6">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="P6">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="Q6">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="R6">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="S6">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="T6">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>144</v>
       </c>
       <c r="U6">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="V6">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>160</v>
       </c>
       <c r="W6">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>168</v>
       </c>
       <c r="X6">
         <f t="shared" si="1"/>
-        <v>92</v>
+        <v>176</v>
       </c>
       <c r="Y6">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>184</v>
       </c>
       <c r="Z6">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>192</v>
       </c>
       <c r="AA6">
         <f t="shared" si="1"/>
-        <v>104</v>
+        <v>200</v>
       </c>
       <c r="AB6">
         <f t="shared" si="1"/>
-        <v>108</v>
+        <v>208</v>
       </c>
       <c r="AC6">
         <f t="shared" si="1"/>
-        <v>112</v>
+        <v>216</v>
       </c>
       <c r="AD6">
         <f t="shared" si="1"/>
-        <v>116</v>
+        <v>224</v>
       </c>
       <c r="AE6">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>232</v>
       </c>
       <c r="AF6">
         <f t="shared" si="1"/>
-        <v>124</v>
+        <v>240</v>
       </c>
       <c r="AG6">
         <f t="shared" si="1"/>
-        <v>128</v>
+        <v>248</v>
       </c>
       <c r="AH6">
         <f t="shared" si="1"/>
-        <v>132</v>
+        <v>256</v>
       </c>
       <c r="AI6">
         <f t="shared" si="1"/>
-        <v>136</v>
+        <v>264</v>
       </c>
       <c r="AJ6">
         <f t="shared" si="1"/>
-        <v>140</v>
+        <v>272</v>
       </c>
       <c r="AK6">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>280</v>
       </c>
       <c r="AL6">
         <f t="shared" si="1"/>
-        <v>148</v>
+        <v>288</v>
       </c>
       <c r="AM6">
         <f t="shared" si="1"/>
-        <v>152</v>
+        <v>296</v>
       </c>
       <c r="AN6">
         <f t="shared" si="1"/>
-        <v>156</v>
+        <v>304</v>
       </c>
       <c r="AO6">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>312</v>
       </c>
       <c r="AP6">
         <f t="shared" si="1"/>
-        <v>164</v>
+        <v>320</v>
       </c>
       <c r="AQ6">
         <f t="shared" si="1"/>
-        <v>168</v>
+        <v>328</v>
       </c>
       <c r="AR6">
         <f t="shared" si="1"/>
-        <v>172</v>
+        <v>336</v>
       </c>
       <c r="AS6">
         <f t="shared" si="1"/>
-        <v>176</v>
+        <v>344</v>
       </c>
       <c r="AT6">
         <f t="shared" si="1"/>
-        <v>180</v>
+        <v>352</v>
       </c>
       <c r="AU6">
         <f t="shared" si="1"/>
-        <v>184</v>
+        <v>360</v>
       </c>
       <c r="AV6">
         <f t="shared" si="1"/>
-        <v>188</v>
+        <v>368</v>
       </c>
       <c r="AW6">
         <f t="shared" si="1"/>
-        <v>192</v>
+        <v>376</v>
       </c>
       <c r="AX6">
         <f t="shared" si="1"/>
-        <v>196</v>
+        <v>384</v>
       </c>
       <c r="AY6">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>392</v>
       </c>
       <c r="AZ6">
         <f t="shared" si="1"/>
-        <v>204</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
@@ -1590,199 +1590,199 @@
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="J7">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="L7">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="M7">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="O7">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="P7">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="Q7">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="R7">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="S7">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="T7">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="U7">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>190</v>
       </c>
       <c r="V7">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>200</v>
       </c>
       <c r="W7">
         <f t="shared" si="1"/>
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="X7">
         <f t="shared" si="1"/>
-        <v>115</v>
+        <v>220</v>
       </c>
       <c r="Y7">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>230</v>
       </c>
       <c r="Z7">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>240</v>
       </c>
       <c r="AA7">
         <f t="shared" si="1"/>
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="AB7">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>260</v>
       </c>
       <c r="AC7">
         <f t="shared" si="1"/>
-        <v>140</v>
+        <v>270</v>
       </c>
       <c r="AD7">
         <f t="shared" si="1"/>
-        <v>145</v>
+        <v>280</v>
       </c>
       <c r="AE7">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>290</v>
       </c>
       <c r="AF7">
         <f t="shared" si="1"/>
-        <v>155</v>
+        <v>300</v>
       </c>
       <c r="AG7">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>310</v>
       </c>
       <c r="AH7">
         <f t="shared" si="1"/>
-        <v>165</v>
+        <v>320</v>
       </c>
       <c r="AI7">
         <f t="shared" si="1"/>
-        <v>170</v>
+        <v>330</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="1"/>
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AK7">
         <f t="shared" si="1"/>
-        <v>180</v>
+        <v>350</v>
       </c>
       <c r="AL7">
         <f t="shared" si="1"/>
-        <v>185</v>
+        <v>360</v>
       </c>
       <c r="AM7">
         <f t="shared" si="1"/>
-        <v>190</v>
+        <v>370</v>
       </c>
       <c r="AN7">
         <f t="shared" si="1"/>
-        <v>195</v>
+        <v>380</v>
       </c>
       <c r="AO7">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>390</v>
       </c>
       <c r="AP7">
         <f t="shared" si="1"/>
-        <v>205</v>
+        <v>400</v>
       </c>
       <c r="AQ7">
         <f t="shared" si="1"/>
-        <v>210</v>
+        <v>410</v>
       </c>
       <c r="AR7">
         <f t="shared" si="1"/>
-        <v>215</v>
+        <v>420</v>
       </c>
       <c r="AS7">
         <f t="shared" si="1"/>
-        <v>220</v>
+        <v>430</v>
       </c>
       <c r="AT7">
         <f t="shared" si="1"/>
-        <v>225</v>
+        <v>440</v>
       </c>
       <c r="AU7">
         <f t="shared" si="1"/>
-        <v>230</v>
+        <v>450</v>
       </c>
       <c r="AV7">
         <f t="shared" si="1"/>
-        <v>235</v>
+        <v>460</v>
       </c>
       <c r="AW7">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>470</v>
       </c>
       <c r="AX7">
         <f t="shared" si="1"/>
-        <v>245</v>
+        <v>480</v>
       </c>
       <c r="AY7">
         <f t="shared" si="1"/>
-        <v>250</v>
+        <v>490</v>
       </c>
       <c r="AZ7">
         <f t="shared" si="1"/>
-        <v>255</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.25">
@@ -1949,203 +1949,203 @@
       </c>
       <c r="C11">
         <f>$B$1*2</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <f>C11+$B$1</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:AZ11" si="3">D11+$B$1</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F11">
         <f>E11+$B$1</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G11">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H11">
         <f t="shared" si="3"/>
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="I11">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="J11">
         <f t="shared" si="3"/>
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="K11">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="L11">
         <f t="shared" si="3"/>
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="M11">
         <f t="shared" si="3"/>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="N11">
         <f t="shared" si="3"/>
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="O11">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="P11">
         <f t="shared" si="3"/>
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="Q11">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="R11">
         <f t="shared" si="3"/>
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="S11">
         <f t="shared" si="3"/>
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="T11">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>190</v>
       </c>
       <c r="U11">
         <f t="shared" si="3"/>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="V11">
         <f t="shared" si="3"/>
-        <v>105</v>
+        <v>210</v>
       </c>
       <c r="W11">
         <f t="shared" si="3"/>
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="X11">
         <f t="shared" si="3"/>
-        <v>115</v>
+        <v>230</v>
       </c>
       <c r="Y11">
         <f t="shared" si="3"/>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="Z11">
         <f t="shared" si="3"/>
-        <v>125</v>
+        <v>250</v>
       </c>
       <c r="AA11">
         <f t="shared" si="3"/>
-        <v>130</v>
+        <v>260</v>
       </c>
       <c r="AB11">
         <f t="shared" si="3"/>
-        <v>135</v>
+        <v>270</v>
       </c>
       <c r="AC11">
         <f t="shared" si="3"/>
-        <v>140</v>
+        <v>280</v>
       </c>
       <c r="AD11">
         <f t="shared" si="3"/>
-        <v>145</v>
+        <v>290</v>
       </c>
       <c r="AE11">
         <f t="shared" si="3"/>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="AF11">
         <f t="shared" si="3"/>
-        <v>155</v>
+        <v>310</v>
       </c>
       <c r="AG11">
         <f t="shared" si="3"/>
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="AH11">
         <f t="shared" si="3"/>
-        <v>165</v>
+        <v>330</v>
       </c>
       <c r="AI11">
         <f t="shared" si="3"/>
-        <v>170</v>
+        <v>340</v>
       </c>
       <c r="AJ11">
         <f t="shared" si="3"/>
-        <v>175</v>
+        <v>350</v>
       </c>
       <c r="AK11">
         <f t="shared" si="3"/>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="AL11">
         <f t="shared" si="3"/>
-        <v>185</v>
+        <v>370</v>
       </c>
       <c r="AM11">
         <f t="shared" si="3"/>
-        <v>190</v>
+        <v>380</v>
       </c>
       <c r="AN11">
         <f t="shared" si="3"/>
-        <v>195</v>
+        <v>390</v>
       </c>
       <c r="AO11">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="AP11">
         <f t="shared" si="3"/>
-        <v>205</v>
+        <v>410</v>
       </c>
       <c r="AQ11">
         <f t="shared" si="3"/>
-        <v>210</v>
+        <v>420</v>
       </c>
       <c r="AR11">
         <f t="shared" si="3"/>
-        <v>215</v>
+        <v>430</v>
       </c>
       <c r="AS11">
         <f t="shared" si="3"/>
-        <v>220</v>
+        <v>440</v>
       </c>
       <c r="AT11">
         <f t="shared" si="3"/>
-        <v>225</v>
+        <v>450</v>
       </c>
       <c r="AU11">
         <f t="shared" si="3"/>
-        <v>230</v>
+        <v>460</v>
       </c>
       <c r="AV11">
         <f t="shared" si="3"/>
-        <v>235</v>
+        <v>470</v>
       </c>
       <c r="AW11">
         <f t="shared" si="3"/>
-        <v>240</v>
+        <v>480</v>
       </c>
       <c r="AX11">
         <f t="shared" si="3"/>
-        <v>245</v>
+        <v>490</v>
       </c>
       <c r="AY11">
         <f t="shared" si="3"/>
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="AZ11">
         <f t="shared" si="3"/>
-        <v>255</v>
+        <v>510</v>
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.25">
@@ -2161,199 +2161,199 @@
       </c>
       <c r="D12">
         <f t="shared" ref="D12:AZ16" si="4">ROUNDUP($A12*D$2,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E12">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F12">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G12">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H12">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I12">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J12">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="K12">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="L12">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="M12">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="N12">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="O12">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="P12">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="Q12">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="R12">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="S12">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="T12">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="U12">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="V12">
         <f t="shared" si="4"/>
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="W12">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="X12">
         <f t="shared" si="4"/>
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="Y12">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="Z12">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="AA12">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="AB12">
         <f t="shared" si="4"/>
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="AC12">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="AD12">
         <f t="shared" si="4"/>
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="AE12">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="AF12">
         <f t="shared" si="4"/>
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="AG12">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="AH12">
         <f t="shared" si="4"/>
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="AI12">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="AJ12">
         <f t="shared" si="4"/>
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="AK12">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="AL12">
         <f t="shared" si="4"/>
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="AM12">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="AN12">
         <f t="shared" si="4"/>
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="AO12">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="AP12">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="AQ12">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="AR12">
         <f t="shared" si="4"/>
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="AS12">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="AT12">
         <f t="shared" si="4"/>
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="AU12">
         <f t="shared" si="4"/>
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="AV12">
         <f t="shared" si="4"/>
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="AW12">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="AX12">
         <f t="shared" si="4"/>
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="AY12">
         <f t="shared" si="4"/>
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="AZ12">
         <f t="shared" si="4"/>
-        <v>51</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.25">
@@ -2369,199 +2369,199 @@
       </c>
       <c r="D13">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E13">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F13">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G13">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H13">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="I13">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="J13">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="K13">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="L13">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="M13">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="N13">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="O13">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="P13">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="Q13">
         <f t="shared" si="5"/>
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="R13">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="S13">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="T13">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="U13">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="V13">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="W13">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="X13">
         <f t="shared" si="4"/>
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="Y13">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="Z13">
         <f t="shared" si="4"/>
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="AA13">
         <f t="shared" si="4"/>
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="AB13">
         <f t="shared" si="4"/>
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="AC13">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="AD13">
         <f t="shared" si="4"/>
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="AE13">
         <f t="shared" si="4"/>
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="AF13">
         <f t="shared" si="4"/>
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="AG13">
         <f t="shared" si="4"/>
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="AH13">
         <f t="shared" si="4"/>
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="AI13">
         <f t="shared" si="4"/>
-        <v>68</v>
+        <v>132</v>
       </c>
       <c r="AJ13">
         <f t="shared" si="4"/>
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="AK13">
         <f t="shared" si="4"/>
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="AL13">
         <f t="shared" si="4"/>
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="AM13">
         <f t="shared" si="4"/>
-        <v>76</v>
+        <v>148</v>
       </c>
       <c r="AN13">
         <f t="shared" si="4"/>
-        <v>78</v>
+        <v>152</v>
       </c>
       <c r="AO13">
         <f t="shared" si="4"/>
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="AP13">
         <f t="shared" si="4"/>
-        <v>82</v>
+        <v>160</v>
       </c>
       <c r="AQ13">
         <f t="shared" si="4"/>
-        <v>84</v>
+        <v>164</v>
       </c>
       <c r="AR13">
         <f t="shared" si="4"/>
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="AS13">
         <f t="shared" si="4"/>
-        <v>88</v>
+        <v>172</v>
       </c>
       <c r="AT13">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>176</v>
       </c>
       <c r="AU13">
         <f t="shared" si="4"/>
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="AV13">
         <f t="shared" si="4"/>
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="AW13">
         <f t="shared" si="4"/>
-        <v>96</v>
+        <v>188</v>
       </c>
       <c r="AX13">
         <f t="shared" si="4"/>
-        <v>98</v>
+        <v>192</v>
       </c>
       <c r="AY13">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>196</v>
       </c>
       <c r="AZ13">
         <f t="shared" si="4"/>
-        <v>102</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.25">
@@ -2577,199 +2577,199 @@
       </c>
       <c r="D14">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E14">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F14">
         <f>ROUNDUP($A14*F$2,0)</f>
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G14">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H14">
         <f t="shared" si="4"/>
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="I14">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="J14">
         <f t="shared" si="4"/>
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="K14">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="L14">
         <f t="shared" si="4"/>
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="M14">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="N14">
         <f t="shared" si="4"/>
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="O14">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="P14">
         <f t="shared" si="4"/>
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="Q14">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="R14">
         <f t="shared" si="4"/>
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="S14">
         <f t="shared" si="4"/>
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="T14">
         <f t="shared" si="4"/>
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="U14">
         <f t="shared" si="4"/>
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="V14">
         <f t="shared" si="4"/>
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="W14">
         <f t="shared" si="4"/>
-        <v>66</v>
+        <v>126</v>
       </c>
       <c r="X14">
         <f t="shared" si="4"/>
-        <v>69</v>
+        <v>132</v>
       </c>
       <c r="Y14">
         <f t="shared" si="4"/>
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="Z14">
         <f t="shared" si="4"/>
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="AA14">
         <f t="shared" si="4"/>
-        <v>78</v>
+        <v>150</v>
       </c>
       <c r="AB14">
         <f t="shared" si="4"/>
-        <v>81</v>
+        <v>156</v>
       </c>
       <c r="AC14">
         <f t="shared" si="4"/>
-        <v>84</v>
+        <v>162</v>
       </c>
       <c r="AD14">
         <f t="shared" si="4"/>
-        <v>87</v>
+        <v>168</v>
       </c>
       <c r="AE14">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>174</v>
       </c>
       <c r="AF14">
         <f t="shared" si="4"/>
-        <v>93</v>
+        <v>180</v>
       </c>
       <c r="AG14">
         <f t="shared" si="4"/>
-        <v>96</v>
+        <v>186</v>
       </c>
       <c r="AH14">
         <f t="shared" si="4"/>
-        <v>99</v>
+        <v>192</v>
       </c>
       <c r="AI14">
         <f t="shared" si="4"/>
-        <v>102</v>
+        <v>198</v>
       </c>
       <c r="AJ14">
         <f t="shared" si="4"/>
-        <v>105</v>
+        <v>204</v>
       </c>
       <c r="AK14">
         <f t="shared" si="4"/>
-        <v>108</v>
+        <v>210</v>
       </c>
       <c r="AL14">
         <f t="shared" si="4"/>
-        <v>111</v>
+        <v>216</v>
       </c>
       <c r="AM14">
         <f t="shared" si="4"/>
-        <v>114</v>
+        <v>222</v>
       </c>
       <c r="AN14">
         <f t="shared" si="4"/>
-        <v>117</v>
+        <v>228</v>
       </c>
       <c r="AO14">
         <f t="shared" si="4"/>
-        <v>120</v>
+        <v>234</v>
       </c>
       <c r="AP14">
         <f t="shared" si="4"/>
-        <v>123</v>
+        <v>240</v>
       </c>
       <c r="AQ14">
         <f t="shared" si="4"/>
-        <v>126</v>
+        <v>246</v>
       </c>
       <c r="AR14">
         <f t="shared" si="4"/>
-        <v>129</v>
+        <v>252</v>
       </c>
       <c r="AS14">
         <f t="shared" si="4"/>
-        <v>132</v>
+        <v>258</v>
       </c>
       <c r="AT14">
         <f t="shared" si="4"/>
-        <v>135</v>
+        <v>264</v>
       </c>
       <c r="AU14">
         <f t="shared" si="4"/>
-        <v>138</v>
+        <v>270</v>
       </c>
       <c r="AV14">
         <f t="shared" si="4"/>
-        <v>141</v>
+        <v>276</v>
       </c>
       <c r="AW14">
         <f t="shared" si="4"/>
-        <v>144</v>
+        <v>282</v>
       </c>
       <c r="AX14">
         <f t="shared" si="4"/>
-        <v>147</v>
+        <v>288</v>
       </c>
       <c r="AY14">
         <f t="shared" si="4"/>
-        <v>150</v>
+        <v>294</v>
       </c>
       <c r="AZ14">
         <f t="shared" si="4"/>
-        <v>153</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.25">
@@ -2785,199 +2785,199 @@
       </c>
       <c r="D15">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E15">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F15">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="G15">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="H15">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="I15">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="J15">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="K15">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="L15">
         <f t="shared" si="4"/>
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="M15">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="N15">
         <f t="shared" si="4"/>
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="O15">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="P15">
         <f t="shared" si="4"/>
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="Q15">
         <f t="shared" si="4"/>
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="R15">
         <f t="shared" si="4"/>
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="S15">
         <f t="shared" si="4"/>
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="T15">
         <f t="shared" si="4"/>
-        <v>76</v>
+        <v>144</v>
       </c>
       <c r="U15">
         <f t="shared" si="4"/>
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="V15">
         <f t="shared" si="4"/>
-        <v>84</v>
+        <v>160</v>
       </c>
       <c r="W15">
         <f t="shared" si="4"/>
-        <v>88</v>
+        <v>168</v>
       </c>
       <c r="X15">
         <f t="shared" si="4"/>
-        <v>92</v>
+        <v>176</v>
       </c>
       <c r="Y15">
         <f t="shared" si="4"/>
-        <v>96</v>
+        <v>184</v>
       </c>
       <c r="Z15">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>192</v>
       </c>
       <c r="AA15">
         <f t="shared" si="4"/>
-        <v>104</v>
+        <v>200</v>
       </c>
       <c r="AB15">
         <f t="shared" si="4"/>
-        <v>108</v>
+        <v>208</v>
       </c>
       <c r="AC15">
         <f t="shared" si="4"/>
-        <v>112</v>
+        <v>216</v>
       </c>
       <c r="AD15">
         <f t="shared" si="4"/>
-        <v>116</v>
+        <v>224</v>
       </c>
       <c r="AE15">
         <f t="shared" si="4"/>
-        <v>120</v>
+        <v>232</v>
       </c>
       <c r="AF15">
         <f t="shared" si="4"/>
-        <v>124</v>
+        <v>240</v>
       </c>
       <c r="AG15">
         <f t="shared" si="4"/>
-        <v>128</v>
+        <v>248</v>
       </c>
       <c r="AH15">
         <f t="shared" si="4"/>
-        <v>132</v>
+        <v>256</v>
       </c>
       <c r="AI15">
         <f t="shared" si="4"/>
-        <v>136</v>
+        <v>264</v>
       </c>
       <c r="AJ15">
         <f t="shared" si="4"/>
-        <v>140</v>
+        <v>272</v>
       </c>
       <c r="AK15">
         <f t="shared" si="4"/>
-        <v>144</v>
+        <v>280</v>
       </c>
       <c r="AL15">
         <f t="shared" si="4"/>
-        <v>148</v>
+        <v>288</v>
       </c>
       <c r="AM15">
         <f t="shared" si="4"/>
-        <v>152</v>
+        <v>296</v>
       </c>
       <c r="AN15">
         <f t="shared" si="4"/>
-        <v>156</v>
+        <v>304</v>
       </c>
       <c r="AO15">
         <f t="shared" si="4"/>
-        <v>160</v>
+        <v>312</v>
       </c>
       <c r="AP15">
         <f t="shared" si="4"/>
-        <v>164</v>
+        <v>320</v>
       </c>
       <c r="AQ15">
         <f t="shared" si="4"/>
-        <v>168</v>
+        <v>328</v>
       </c>
       <c r="AR15">
         <f t="shared" si="4"/>
-        <v>172</v>
+        <v>336</v>
       </c>
       <c r="AS15">
         <f t="shared" si="4"/>
-        <v>176</v>
+        <v>344</v>
       </c>
       <c r="AT15">
         <f t="shared" si="4"/>
-        <v>180</v>
+        <v>352</v>
       </c>
       <c r="AU15">
         <f t="shared" si="4"/>
-        <v>184</v>
+        <v>360</v>
       </c>
       <c r="AV15">
         <f t="shared" si="4"/>
-        <v>188</v>
+        <v>368</v>
       </c>
       <c r="AW15">
         <f t="shared" si="4"/>
-        <v>192</v>
+        <v>376</v>
       </c>
       <c r="AX15">
         <f t="shared" si="4"/>
-        <v>196</v>
+        <v>384</v>
       </c>
       <c r="AY15">
         <f t="shared" si="4"/>
-        <v>200</v>
+        <v>392</v>
       </c>
       <c r="AZ15">
         <f t="shared" si="4"/>
-        <v>204</v>
+        <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.25">
@@ -2993,199 +2993,199 @@
       </c>
       <c r="D16">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E16">
         <f>ROUNDUP($A16*E$2,0)</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F16">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G16">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H16">
         <f t="shared" si="4"/>
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="I16">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="J16">
         <f t="shared" si="4"/>
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="K16">
         <f t="shared" si="4"/>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="L16">
         <f t="shared" si="4"/>
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="M16">
         <f t="shared" si="4"/>
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="N16">
         <f t="shared" si="4"/>
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="O16">
         <f t="shared" si="4"/>
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="P16">
         <f t="shared" si="4"/>
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="Q16">
         <f t="shared" si="4"/>
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="R16">
         <f t="shared" si="4"/>
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="S16">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="T16">
         <f t="shared" si="4"/>
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="U16">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>190</v>
       </c>
       <c r="V16">
         <f t="shared" si="4"/>
-        <v>105</v>
+        <v>200</v>
       </c>
       <c r="W16">
         <f t="shared" si="4"/>
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="X16">
         <f t="shared" si="4"/>
-        <v>115</v>
+        <v>220</v>
       </c>
       <c r="Y16">
         <f t="shared" si="4"/>
-        <v>120</v>
+        <v>230</v>
       </c>
       <c r="Z16">
         <f t="shared" si="4"/>
-        <v>125</v>
+        <v>240</v>
       </c>
       <c r="AA16">
         <f t="shared" si="4"/>
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="AB16">
         <f t="shared" si="4"/>
-        <v>135</v>
+        <v>260</v>
       </c>
       <c r="AC16">
         <f t="shared" si="4"/>
-        <v>140</v>
+        <v>270</v>
       </c>
       <c r="AD16">
         <f t="shared" si="4"/>
-        <v>145</v>
+        <v>280</v>
       </c>
       <c r="AE16">
         <f t="shared" si="4"/>
-        <v>150</v>
+        <v>290</v>
       </c>
       <c r="AF16">
         <f t="shared" si="4"/>
-        <v>155</v>
+        <v>300</v>
       </c>
       <c r="AG16">
         <f t="shared" si="4"/>
-        <v>160</v>
+        <v>310</v>
       </c>
       <c r="AH16">
         <f t="shared" si="4"/>
-        <v>165</v>
+        <v>320</v>
       </c>
       <c r="AI16">
         <f t="shared" si="4"/>
-        <v>170</v>
+        <v>330</v>
       </c>
       <c r="AJ16">
         <f t="shared" si="4"/>
-        <v>175</v>
+        <v>340</v>
       </c>
       <c r="AK16">
         <f t="shared" si="4"/>
-        <v>180</v>
+        <v>350</v>
       </c>
       <c r="AL16">
         <f t="shared" si="4"/>
-        <v>185</v>
+        <v>360</v>
       </c>
       <c r="AM16">
         <f t="shared" si="4"/>
-        <v>190</v>
+        <v>370</v>
       </c>
       <c r="AN16">
         <f t="shared" si="4"/>
-        <v>195</v>
+        <v>380</v>
       </c>
       <c r="AO16">
         <f t="shared" si="4"/>
-        <v>200</v>
+        <v>390</v>
       </c>
       <c r="AP16">
         <f t="shared" si="4"/>
-        <v>205</v>
+        <v>400</v>
       </c>
       <c r="AQ16">
         <f t="shared" si="4"/>
-        <v>210</v>
+        <v>410</v>
       </c>
       <c r="AR16">
         <f t="shared" si="4"/>
-        <v>215</v>
+        <v>420</v>
       </c>
       <c r="AS16">
         <f t="shared" si="4"/>
-        <v>220</v>
+        <v>430</v>
       </c>
       <c r="AT16">
         <f t="shared" si="4"/>
-        <v>225</v>
+        <v>440</v>
       </c>
       <c r="AU16">
         <f t="shared" si="4"/>
-        <v>230</v>
+        <v>450</v>
       </c>
       <c r="AV16">
         <f t="shared" si="4"/>
-        <v>235</v>
+        <v>460</v>
       </c>
       <c r="AW16">
         <f t="shared" si="4"/>
-        <v>240</v>
+        <v>470</v>
       </c>
       <c r="AX16">
         <f t="shared" si="4"/>
-        <v>245</v>
+        <v>480</v>
       </c>
       <c r="AY16">
         <f t="shared" si="4"/>
-        <v>250</v>
+        <v>490</v>
       </c>
       <c r="AZ16">
         <f t="shared" si="4"/>
-        <v>255</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>